<commit_message>
script with NER validation
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Documents\01_dev\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E05FF4-18E4-4F0B-8157-480DA99A0224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAA5DE5-4104-40B4-A7EB-F99449D179B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>poradie</t>
+    <t>Entry</t>
   </si>
   <si>
-    <t>meno:</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>filename:</t>
+    <t>Filename</t>
   </si>
 </sst>
 </file>
@@ -394,10 +394,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="A2:D20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="37.3671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">

</xml_diff>